<commit_message>
ATUALIZAÇÃO ERP SUZUKI - VERSÃO 2.04.000 - 02/09/2024
</commit_message>
<xml_diff>
--- a/arquivos/modelo excel/ov_incluir.xlsx
+++ b/arquivos/modelo excel/ov_incluir.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anderson\PycharmProjects\erp_suzuki\arquivos\modelo excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anderson\PycharmProjects\menu_teste\arquivos\modelo excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0061709-4189-404B-BCC8-A9D24E633074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C962104-4F90-45D7-AA9E-54BED38BC982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,16 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -51,9 +41,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Data Necessária</t>
   </si>
   <si>
     <t>Observações</t>
@@ -231,6 +218,9 @@
   </si>
   <si>
     <t>Ipi %</t>
+  </si>
+  <si>
+    <t>Previsão de Entrega</t>
   </si>
 </sst>
 </file>
@@ -755,7 +745,7 @@
   <dimension ref="A2:N1012"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,7 +764,7 @@
   <sheetData>
     <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C2" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
@@ -790,39 +780,39 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="15"/>
       <c r="F4" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="J4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C5" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="15"/>
       <c r="F5" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="J5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="15"/>
       <c r="F6" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -868,16 +858,16 @@
         <v>5</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>